<commit_message>
Implemented opening different windows
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marek\Documents\GitHub\small_rpg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35795B0F-266A-4362-B51B-4915584481B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EF70A5-8036-4F2C-9458-D1F20DCD9CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{6C8063F9-2533-4B6A-8DC9-0AE75D53401A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{6C8063F9-2533-4B6A-8DC9-0AE75D53401A}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -2389,7 +2389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B18085-8321-4901-8675-3744BC5E2226}">
   <dimension ref="B1:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
@@ -2643,8 +2643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8E6549-6574-4F90-A35D-AE6E56F6B7A0}">
   <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3318,7 +3318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A94EA5-FE59-49DA-9957-5EF33B1E2378}">
   <dimension ref="B1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added base skill class
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marek\Documents\GitHub\small_rpg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VW2SMDW\Repos\small_rpg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EF70A5-8036-4F2C-9458-D1F20DCD9CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF13610D-051A-4E6E-AEF9-ED449D0616E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{6C8063F9-2533-4B6A-8DC9-0AE75D53401A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{6C8063F9-2533-4B6A-8DC9-0AE75D53401A}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="181">
   <si>
     <t>Barbarian</t>
   </si>
@@ -520,9 +520,6 @@
     <t>Legalize Nuclear Bombs</t>
   </si>
   <si>
-    <t>Drops a literal Nuke on the Enemy, dealing every Damage type</t>
-  </si>
-  <si>
     <t>Skill</t>
   </si>
   <si>
@@ -553,16 +550,40 @@
     <t>Raise Attack forgetts Debuffs (still happen but not in stat bar), Damage Numbers and own Health makes no Sense</t>
   </si>
   <si>
-    <t>Tard Strength</t>
-  </si>
-  <si>
     <t>Reanimate every Fallen Party Member and Lower Enemies for 3 Turns, Reanimated Thralls cannot Die in that Time. After 3 Turns they die again and cannot be reanimated or ressurected for 5 Turns. If no Teammate is dead, Summon 3 lvl.50 Thralls</t>
   </si>
   <si>
-    <t>Every Attack deals AOE Damage for 10 Turns, Splash Damage According to Enemy Placement</t>
-  </si>
-  <si>
-    <t>Only Available at -5 Intelligence</t>
+    <t>Primal Rage</t>
+  </si>
+  <si>
+    <t>After 5 Turns Ursoid becomes Feral and wont take commands. Will Attack everyone including Allies</t>
+  </si>
+  <si>
+    <t>Wonders of the Universe</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Every Attack deals AOE Damage for 10 Turns, Splash Damage According to Enemy Placement. Damage Scales with negative Intelligence</t>
+  </si>
+  <si>
+    <t>"The Unisverse it sings to Us. Witness its beauty. Inspire your Allies and Damage your Enemies with the Power of the Universe</t>
+  </si>
+  <si>
+    <t>Buff Attack and Defence of Allies. Damage Enemies with two Colliding Universes</t>
+  </si>
+  <si>
+    <t>"GURAAAAH". Enchance your Power but be careful of its Duration. Or you may hurt your Allies more than your Enemies</t>
+  </si>
+  <si>
+    <t>Drops a literal Nuke on the Enemy, dealing every Damage type. 2 Turn Charge Up First turn needs DreamyBull "Imbouttoblow" second needs "LEGALIZE NUCLEAR BOMBS"</t>
+  </si>
+  <si>
+    <t>"CALL THE FIRE DEPARTMENT CAUSE WE JUST NUKED THE BUILDING" Drop A Nuke damaging everone on the Field with every elemental Damage Type</t>
+  </si>
+  <si>
+    <t>"I am the way into the city of woe, I am the way into eternal pain, I am the way to go among the lost." Take your Enemie through the 9 Stages of Hell. Every Turn does a different Debuff. While you, yourself, arent Protected from ist Effects</t>
   </si>
 </sst>
 </file>
@@ -2636,6 +2657,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Arial"&amp;8&amp;K000000INTERNAL&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2643,7 +2668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8E6549-6574-4F90-A35D-AE6E56F6B7A0}">
   <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8:C10"/>
     </sheetView>
   </sheetViews>
@@ -2850,7 +2875,7 @@
         <v>51</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>72</v>
@@ -2907,7 +2932,7 @@
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8" t="s">
@@ -2923,14 +2948,14 @@
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H2" s="9"/>
       <c r="K2" s="8"/>
@@ -3137,13 +3162,13 @@
     </row>
     <row r="17" spans="4:16" ht="75" x14ac:dyDescent="0.25">
       <c r="D17" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="F17" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="G17" s="9" t="s">
         <v>167</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>168</v>
       </c>
       <c r="H17" s="9"/>
       <c r="K17" s="8"/>
@@ -3316,68 +3341,73 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A94EA5-FE59-49DA-9957-5EF33B1E2378}">
-  <dimension ref="B1:G9"/>
+  <dimension ref="B1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="1"/>
-    <col min="6" max="6" width="35.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="34" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="34"/>
+    <col min="6" max="6" width="35.28515625" style="34" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" style="34" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="34"/>
+    <col min="9" max="9" width="53.5703125" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="34" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="I1" s="34" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="120" x14ac:dyDescent="0.25">
       <c r="B3" s="34" t="s">
         <v>152</v>
       </c>
       <c r="D3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="34"/>
       <c r="F3" s="34" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G3" s="34" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="105" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="C5" s="34"/>
       <c r="D5" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="34"/>
       <c r="F5" s="34" t="s">
         <v>157</v>
       </c>
       <c r="G5" s="34" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="I5" s="34" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>158</v>
       </c>
@@ -3387,28 +3417,52 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I7" s="34" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B9" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="I9" s="34" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>173</v>
+      <c r="D11" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="I11" s="34" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Arial"&amp;8&amp;K000000INTERNAL&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -3471,7 +3525,7 @@
         <v>89</v>
       </c>
       <c r="J6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K6" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
added first map draft
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VW2SMDW\Repos\small_rpg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marek\Documents\GitHub\small_rpg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF13610D-051A-4E6E-AEF9-ED449D0616E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECD9BA4-F210-4472-8C96-714978747F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{6C8063F9-2533-4B6A-8DC9-0AE75D53401A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{6C8063F9-2533-4B6A-8DC9-0AE75D53401A}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="182">
   <si>
     <t>Barbarian</t>
   </si>
@@ -211,9 +211,6 @@
     <t>Devil</t>
   </si>
   <si>
-    <t>Suc-/Incubus</t>
-  </si>
-  <si>
     <t>Lich</t>
   </si>
   <si>
@@ -226,21 +223,12 @@
     <t>Fire Buff on all attacks</t>
   </si>
   <si>
-    <t>Lower Damage to same Sex</t>
-  </si>
-  <si>
     <t>Higher Damage from Light</t>
   </si>
   <si>
-    <t>unable to use ice magic</t>
-  </si>
-  <si>
     <t>Demon Lord</t>
   </si>
   <si>
-    <t>Seductress (High Priest)</t>
-  </si>
-  <si>
     <t>Demon Lord (Grand Knight)</t>
   </si>
   <si>
@@ -584,6 +572,21 @@
   </si>
   <si>
     <t>"I am the way into the city of woe, I am the way into eternal pain, I am the way to go among the lost." Take your Enemie through the 9 Stages of Hell. Every Turn does a different Debuff. While you, yourself, arent Protected from ist Effects</t>
+  </si>
+  <si>
+    <t>Judicor</t>
+  </si>
+  <si>
+    <t>Banshee</t>
+  </si>
+  <si>
+    <t>Bard (High Priest)</t>
+  </si>
+  <si>
+    <t>Bard</t>
+  </si>
+  <si>
+    <t>Celebrity</t>
   </si>
 </sst>
 </file>
@@ -1128,7 +1131,7 @@
   <dimension ref="B3:AO25"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1174,7 @@
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
       <c r="D3" s="14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E3" s="15" t="s">
         <v>17</v>
@@ -1180,23 +1183,23 @@
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
       <c r="K3" s="20" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="M3" s="22" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="N3" s="23" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="O3" s="21"/>
       <c r="P3" s="24" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="Q3" s="25" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="R3" s="21"/>
       <c r="S3" s="26" t="s">
@@ -1255,18 +1258,18 @@
       <c r="B4" s="14"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="14"/>
       <c r="K4" s="20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="L4" s="21"/>
       <c r="M4" s="22"/>
@@ -1308,17 +1311,17 @@
       <c r="G5" s="2"/>
       <c r="H5" s="14"/>
       <c r="J5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="L5" s="21"/>
       <c r="M5" s="22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="N5" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="O5" s="21"/>
       <c r="P5" s="24"/>
@@ -1339,15 +1342,15 @@
       <c r="AE5" s="21"/>
       <c r="AF5" s="20"/>
       <c r="AG5" s="22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AH5" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AI5" s="21"/>
       <c r="AJ5" s="24"/>
       <c r="AK5" s="25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AL5" s="21"/>
       <c r="AM5" s="26"/>
@@ -1359,23 +1362,23 @@
       <c r="C6" s="14"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="J6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="L6" s="21"/>
       <c r="M6" s="22"/>
       <c r="N6" s="23"/>
       <c r="O6" s="21"/>
       <c r="P6" s="24" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="Q6" s="25"/>
       <c r="R6" s="21"/>
@@ -1405,38 +1408,40 @@
     </row>
     <row r="7" spans="2:41" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="14"/>
       <c r="F7" s="2"/>
       <c r="G7" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="14"/>
+        <v>63</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>177</v>
+      </c>
       <c r="J7" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="L7" s="21"/>
       <c r="M7" s="22"/>
       <c r="N7" s="23"/>
       <c r="O7" s="21"/>
       <c r="P7" s="24" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="Q7" s="25"/>
       <c r="R7" s="21"/>
       <c r="S7" s="26" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="T7" s="27" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="U7" s="21"/>
       <c r="V7" s="20"/>
@@ -1444,10 +1449,10 @@
       <c r="X7" s="23"/>
       <c r="Y7" s="21"/>
       <c r="Z7" s="24" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AA7" s="25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AB7" s="21"/>
       <c r="AC7" s="26"/>
@@ -1472,9 +1477,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="13" t="s">
-        <v>3</v>
-      </c>
+      <c r="E8" s="13"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5" t="s">
         <v>2</v>
@@ -1483,10 +1486,10 @@
         <v>18</v>
       </c>
       <c r="J8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="L8" s="21"/>
       <c r="M8" s="22"/>
@@ -1510,17 +1513,17 @@
       <c r="AE8" s="21"/>
       <c r="AF8" s="20"/>
       <c r="AG8" s="22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AH8" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AI8" s="21"/>
       <c r="AJ8" s="24" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AK8" s="25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AL8" s="21"/>
       <c r="AM8" s="26"/>
@@ -1536,27 +1539,27 @@
       <c r="G9" s="2"/>
       <c r="H9" s="14"/>
       <c r="J9" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K9" s="20" t="s">
         <v>29</v>
       </c>
       <c r="L9" s="21"/>
       <c r="M9" s="22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="N9" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="O9" s="21"/>
       <c r="P9" s="24"/>
       <c r="Q9" s="25"/>
       <c r="R9" s="21"/>
       <c r="S9" s="26" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="T9" s="27" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="U9" s="21"/>
       <c r="V9" s="20"/>
@@ -1584,7 +1587,7 @@
       <c r="B10" s="14"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>21</v>
@@ -1593,25 +1596,25 @@
       <c r="G10" s="2"/>
       <c r="H10" s="14"/>
       <c r="J10" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L10" s="21"/>
       <c r="M10" s="22"/>
       <c r="N10" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="24"/>
       <c r="Q10" s="25"/>
       <c r="R10" s="21"/>
       <c r="S10" s="26" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="T10" s="27" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="U10" s="21"/>
       <c r="V10" s="20"/>
@@ -1639,7 +1642,7 @@
       <c r="B11" s="14"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>5</v>
@@ -1688,22 +1691,22 @@
       <c r="G12" s="2"/>
       <c r="H12" s="14"/>
       <c r="J12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="L12" s="21"/>
       <c r="M12" s="22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="O12" s="21"/>
       <c r="P12" s="24"/>
       <c r="Q12" s="25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="R12" s="21"/>
       <c r="S12" s="26"/>
@@ -1741,20 +1744,20 @@
       <c r="G13" s="2"/>
       <c r="H13" s="14"/>
       <c r="J13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="L13" s="21"/>
       <c r="M13" s="22"/>
       <c r="N13" s="23"/>
       <c r="O13" s="21"/>
       <c r="P13" s="24" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="Q13" s="25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="R13" s="21"/>
       <c r="S13" s="26"/>
@@ -1786,20 +1789,22 @@
         <v>41</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>180</v>
+      </c>
       <c r="H14" s="14" t="s">
-        <v>90</v>
+        <v>181</v>
       </c>
       <c r="J14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="L14" s="21"/>
       <c r="M14" s="22"/>
@@ -1807,12 +1812,12 @@
       <c r="O14" s="21"/>
       <c r="P14" s="24"/>
       <c r="Q14" s="25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="R14" s="21"/>
       <c r="S14" s="26"/>
       <c r="T14" s="27" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="U14" s="21"/>
       <c r="V14" s="20"/>
@@ -1847,13 +1852,13 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H15" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K15" s="20" t="s">
         <v>31</v>
@@ -1886,10 +1891,10 @@
       <c r="AK15" s="25"/>
       <c r="AL15" s="21"/>
       <c r="AM15" s="26" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AN15" s="27" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AO15" s="21"/>
     </row>
@@ -1902,10 +1907,10 @@
       <c r="G16" s="2"/>
       <c r="H16" s="14"/>
       <c r="J16" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K16" s="20" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="L16" s="21"/>
       <c r="M16" s="22"/>
@@ -1935,10 +1940,10 @@
       <c r="AK16" s="25"/>
       <c r="AL16" s="21"/>
       <c r="AM16" s="26" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AN16" s="27" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AO16" s="21"/>
     </row>
@@ -1946,7 +1951,7 @@
       <c r="B17" s="14"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>22</v>
@@ -1955,10 +1960,10 @@
       <c r="G17" s="2"/>
       <c r="H17" s="14"/>
       <c r="J17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="L17" s="21"/>
       <c r="M17" s="22"/>
@@ -1983,14 +1988,14 @@
       <c r="AF17" s="20"/>
       <c r="AG17" s="22"/>
       <c r="AH17" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AI17" s="21"/>
       <c r="AJ17" s="24" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AK17" s="25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AL17" s="21"/>
       <c r="AM17" s="26"/>
@@ -2001,7 +2006,7 @@
       <c r="B18" s="14"/>
       <c r="C18" s="10"/>
       <c r="D18" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>10</v>
@@ -2010,20 +2015,20 @@
       <c r="G18" s="6"/>
       <c r="H18" s="14"/>
       <c r="J18" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L18" s="21"/>
       <c r="M18" s="22"/>
       <c r="N18" s="23"/>
       <c r="O18" s="21"/>
       <c r="P18" s="24" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="Q18" s="25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="R18" s="21"/>
       <c r="S18" s="26"/>
@@ -2032,7 +2037,7 @@
       <c r="V18" s="20"/>
       <c r="W18" s="22"/>
       <c r="X18" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="Y18" s="21"/>
       <c r="Z18" s="24"/>
@@ -2043,17 +2048,17 @@
       <c r="AE18" s="21"/>
       <c r="AF18" s="20"/>
       <c r="AG18" s="22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AH18" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AI18" s="21"/>
       <c r="AJ18" s="24" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AK18" s="25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AL18" s="21"/>
       <c r="AM18" s="26"/>
@@ -2111,7 +2116,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="14"/>
       <c r="K20" s="20" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="L20" s="21"/>
       <c r="M20" s="22"/>
@@ -2146,29 +2151,29 @@
     </row>
     <row r="21" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K21" s="20" t="s">
         <v>25</v>
       </c>
       <c r="L21" s="21"/>
       <c r="M21" s="22" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="N21" s="23" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="O21" s="21"/>
       <c r="P21" s="24"/>
@@ -2179,17 +2184,17 @@
       <c r="U21" s="21"/>
       <c r="V21" s="20"/>
       <c r="W21" s="22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="X21" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="Y21" s="21"/>
       <c r="Z21" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA21" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB21" s="21"/>
       <c r="AC21" s="26"/>
@@ -2237,15 +2242,15 @@
       <c r="U22" s="21"/>
       <c r="V22" s="20"/>
       <c r="W22" s="22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="X22" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="Y22" s="21"/>
       <c r="Z22" s="24"/>
       <c r="AA22" s="25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AB22" s="21"/>
       <c r="AC22" s="26"/>
@@ -2264,7 +2269,7 @@
     </row>
     <row r="23" spans="2:41" x14ac:dyDescent="0.25">
       <c r="K23" s="20" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="L23" s="21"/>
       <c r="M23" s="22"/>
@@ -2278,10 +2283,10 @@
       <c r="U23" s="21"/>
       <c r="V23" s="20"/>
       <c r="W23" s="22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="X23" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="Y23" s="21"/>
       <c r="Z23" s="24"/>
@@ -2289,7 +2294,7 @@
       <c r="AB23" s="21"/>
       <c r="AC23" s="26"/>
       <c r="AD23" s="27" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AE23" s="21"/>
       <c r="AF23" s="20"/>
@@ -2315,10 +2320,10 @@
       <c r="Q24" s="25"/>
       <c r="R24" s="21"/>
       <c r="S24" s="26" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="T24" s="27" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="U24" s="21"/>
       <c r="V24" s="20"/>
@@ -2329,10 +2334,10 @@
       <c r="AA24" s="25"/>
       <c r="AB24" s="21"/>
       <c r="AC24" s="26" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AD24" s="27" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AE24" s="21"/>
       <c r="AF24" s="20"/>
@@ -2343,10 +2348,10 @@
       <c r="AK24" s="25"/>
       <c r="AL24" s="21"/>
       <c r="AM24" s="26" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AN24" s="27" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AO24" s="21"/>
     </row>
@@ -2369,28 +2374,28 @@
       <c r="X25" s="23"/>
       <c r="Y25" s="21"/>
       <c r="Z25" s="24" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AA25" s="25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AB25" s="21"/>
       <c r="AC25" s="26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="AD25" s="27" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="AE25" s="21"/>
       <c r="AF25" s="20"/>
       <c r="AG25" s="22"/>
       <c r="AH25" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AI25" s="21"/>
       <c r="AJ25" s="24"/>
       <c r="AK25" s="25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AL25" s="21"/>
       <c r="AM25" s="26"/>
@@ -2410,7 +2415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B18085-8321-4901-8675-3744BC5E2226}">
   <dimension ref="B1:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
@@ -2422,12 +2427,12 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -2437,7 +2442,7 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -2447,7 +2452,7 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -2455,7 +2460,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
@@ -2463,15 +2468,15 @@
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -2479,15 +2484,15 @@
         <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -2495,7 +2500,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -2503,15 +2508,15 @@
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -2521,18 +2526,18 @@
     </row>
     <row r="20" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G24" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
@@ -2540,15 +2545,15 @@
         <v>5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -2556,15 +2561,15 @@
         <v>21</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -2572,7 +2577,7 @@
         <v>14</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -2580,15 +2585,15 @@
         <v>8</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="45" x14ac:dyDescent="0.25">
@@ -2596,7 +2601,7 @@
         <v>20</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -2604,7 +2609,7 @@
         <v>41</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="60" x14ac:dyDescent="0.25">
@@ -2612,7 +2617,7 @@
         <v>16</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
@@ -2620,15 +2625,15 @@
         <v>7</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -2636,15 +2641,15 @@
         <v>13</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="45" x14ac:dyDescent="0.25">
@@ -2652,7 +2657,7 @@
         <v>15</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2669,7 +2674,7 @@
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C10"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2730,13 +2735,13 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -2782,38 +2787,34 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>56</v>
+        <v>178</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>65</v>
+        <v>179</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>61</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
       <c r="C10" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2821,10 +2822,10 @@
         <v>42</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -2856,10 +2857,10 @@
         <v>52</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -2875,10 +2876,10 @@
         <v>51</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -2892,10 +2893,10 @@
         <v>54</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2932,30 +2933,30 @@
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="2:18" ht="60" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H2" s="9"/>
       <c r="K2" s="8"/>
@@ -3146,7 +3147,7 @@
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -3162,13 +3163,13 @@
     </row>
     <row r="17" spans="4:16" ht="75" x14ac:dyDescent="0.25">
       <c r="D17" s="33" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H17" s="9"/>
       <c r="K17" s="8"/>
@@ -3361,100 +3362,100 @@
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" s="34" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="120" x14ac:dyDescent="0.25">
       <c r="B3" s="34" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D3" s="34" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="105" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="I5" s="34" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I7" s="34" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B9" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" s="34" t="s">
-        <v>174</v>
-      </c>
       <c r="G9" s="34" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="I9" s="34" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="34" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D11" s="34" t="s">
         <v>21</v>
       </c>
       <c r="F11" s="34" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I11" s="34" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -3481,16 +3482,16 @@
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G2" t="s">
         <v>30</v>
@@ -3499,36 +3500,36 @@
         <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" t="s">
         <v>82</v>
       </c>
-      <c r="E6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" t="s">
-        <v>86</v>
-      </c>
       <c r="G6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H6" t="s">
         <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="K6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>